<commit_message>
Fusion des motifs Grande surface et Commerces de proximite
</commit_message>
<xml_diff>
--- a/mobility/data/insee/esane/equipments_features.xlsx
+++ b/mobility/data/insee/esane/equipments_features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauchota\Documents\repo_mobility\mobility\data\insee\esane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB60C686-26F4-4A8D-9FD6-931F99823343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B10ED2-B2F2-463C-89EC-EE25D26F4F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12768" yWindow="4008" windowWidth="17280" windowHeight="8964" xr2:uid="{76399115-CEC3-4B1F-8B90-B75E677355CC}"/>
+    <workbookView xWindow="13188" yWindow="2052" windowWidth="17280" windowHeight="8964" xr2:uid="{76399115-CEC3-4B1F-8B90-B75E677355CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="292">
   <si>
     <t>shop_area</t>
   </si>
@@ -888,12 +888,6 @@
     <t>motive_label</t>
   </si>
   <si>
-    <t>Se rendre dans une grande surface ou un centre commercial (y compris boutiques et services)</t>
-  </si>
-  <si>
-    <t>Se rendre dans un centre de proximité, petit commerce, supérette, boutique, services (banque, cordonnier...) commercial) (hors centre commercial)</t>
-  </si>
-  <si>
     <t>Étudier (école, lycée, université)</t>
   </si>
   <si>
@@ -913,6 +907,9 @@
   </si>
   <si>
     <t>Manger ou boire à l’extérieur du domicile</t>
+  </si>
+  <si>
+    <t>Commerce</t>
   </si>
 </sst>
 </file>
@@ -1279,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DE583F-5E34-4D85-83E5-ED5AB884D896}">
   <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1318,10 +1315,10 @@
         <v>52</v>
       </c>
       <c r="C2" s="1">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E2">
         <v>6000</v>
@@ -1335,10 +1332,10 @@
         <v>53</v>
       </c>
       <c r="C3" s="1">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E3">
         <v>1000</v>
@@ -1352,10 +1349,10 @@
         <v>54</v>
       </c>
       <c r="C4" s="1">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1366,10 +1363,10 @@
         <v>55</v>
       </c>
       <c r="C5" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="E5">
         <v>200</v>
@@ -1383,14 +1380,12 @@
         <v>56</v>
       </c>
       <c r="C6" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>285</v>
-      </c>
-      <c r="F6" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1400,14 +1395,12 @@
         <v>57</v>
       </c>
       <c r="C7" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>285</v>
-      </c>
-      <c r="F7" s="1">
-        <v>200</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1417,14 +1410,12 @@
         <v>58</v>
       </c>
       <c r="C8" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>285</v>
-      </c>
-      <c r="F8" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1434,14 +1425,12 @@
         <v>59</v>
       </c>
       <c r="C9" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>285</v>
-      </c>
-      <c r="F9" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1451,14 +1440,12 @@
         <v>60</v>
       </c>
       <c r="C10" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>285</v>
-      </c>
-      <c r="F10" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1468,14 +1455,12 @@
         <v>61</v>
       </c>
       <c r="C11" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>285</v>
-      </c>
-      <c r="F11" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1485,14 +1470,12 @@
         <v>63</v>
       </c>
       <c r="C12" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>285</v>
-      </c>
-      <c r="F12" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1502,14 +1485,12 @@
         <v>65</v>
       </c>
       <c r="C13" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>285</v>
-      </c>
-      <c r="F13" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1519,14 +1500,12 @@
         <v>67</v>
       </c>
       <c r="C14" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>285</v>
-      </c>
-      <c r="F14" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1536,14 +1515,12 @@
         <v>69</v>
       </c>
       <c r="C15" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>285</v>
-      </c>
-      <c r="F15" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1553,14 +1530,12 @@
         <v>71</v>
       </c>
       <c r="C16" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>285</v>
-      </c>
-      <c r="F16" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -1570,14 +1545,12 @@
         <v>73</v>
       </c>
       <c r="C17" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>285</v>
-      </c>
-      <c r="F17" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1587,14 +1560,12 @@
         <v>75</v>
       </c>
       <c r="C18" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>285</v>
-      </c>
-      <c r="F18" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -1604,14 +1575,12 @@
         <v>77</v>
       </c>
       <c r="C19" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>285</v>
-      </c>
-      <c r="F19" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -1621,14 +1590,12 @@
         <v>79</v>
       </c>
       <c r="C20" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>285</v>
-      </c>
-      <c r="F20" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1638,14 +1605,12 @@
         <v>81</v>
       </c>
       <c r="C21" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>285</v>
-      </c>
-      <c r="F21" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1655,14 +1620,12 @@
         <v>83</v>
       </c>
       <c r="C22" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>285</v>
-      </c>
-      <c r="F22" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1672,14 +1635,12 @@
         <v>85</v>
       </c>
       <c r="C23" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>285</v>
-      </c>
-      <c r="F23" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1689,14 +1650,12 @@
         <v>87</v>
       </c>
       <c r="C24" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>285</v>
-      </c>
-      <c r="F24" s="1">
-        <v>50</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1706,14 +1665,12 @@
         <v>89</v>
       </c>
       <c r="C25" s="1">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>285</v>
-      </c>
-      <c r="F25" s="1">
-        <v>100</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1726,7 +1683,7 @@
         <v>1.4</v>
       </c>
       <c r="D26" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F26" s="1">
         <v>60</v>
@@ -1743,7 +1700,7 @@
         <v>1.4</v>
       </c>
       <c r="D27" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F27" s="1">
         <v>20</v>
@@ -1760,7 +1717,7 @@
         <v>1.4</v>
       </c>
       <c r="D28" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F28" s="1">
         <v>200</v>
@@ -1777,7 +1734,7 @@
         <v>1.4</v>
       </c>
       <c r="D29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F29" s="1">
         <v>70</v>
@@ -1794,7 +1751,7 @@
         <v>1.4</v>
       </c>
       <c r="D30" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F30" s="1">
         <v>600</v>
@@ -1811,7 +1768,7 @@
         <v>1.4</v>
       </c>
       <c r="D31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F31" s="1">
         <v>500</v>
@@ -1828,7 +1785,7 @@
         <v>1.4</v>
       </c>
       <c r="D32" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F32" s="1">
         <v>200</v>
@@ -1845,7 +1802,7 @@
         <v>1.4</v>
       </c>
       <c r="D33" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F33" s="1">
         <v>200</v>
@@ -1862,7 +1819,7 @@
         <v>1.4</v>
       </c>
       <c r="D34" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F34" s="1">
         <v>50</v>
@@ -1879,7 +1836,7 @@
         <v>1.4</v>
       </c>
       <c r="D35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F35" s="1">
         <v>50</v>
@@ -1896,7 +1853,7 @@
         <v>1.4</v>
       </c>
       <c r="D36" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F36" s="1">
         <v>200</v>
@@ -1913,7 +1870,7 @@
         <v>1.4</v>
       </c>
       <c r="D37" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F37" s="1">
         <v>200</v>
@@ -1930,7 +1887,7 @@
         <v>1.4</v>
       </c>
       <c r="D38" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F38" s="1">
         <v>200</v>
@@ -1947,7 +1904,7 @@
         <v>1.4</v>
       </c>
       <c r="D39" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F39" s="1">
         <v>50</v>
@@ -1964,7 +1921,7 @@
         <v>1.4</v>
       </c>
       <c r="D40" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F40" s="1">
         <v>50</v>
@@ -1981,7 +1938,7 @@
         <v>1.4</v>
       </c>
       <c r="D41" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F41" s="1">
         <v>500</v>
@@ -1998,7 +1955,7 @@
         <v>1.4</v>
       </c>
       <c r="D42" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F42" s="1">
         <v>200</v>
@@ -2015,7 +1972,7 @@
         <v>1.4</v>
       </c>
       <c r="D43" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F43" s="1">
         <v>50</v>
@@ -2032,7 +1989,7 @@
         <v>1.4</v>
       </c>
       <c r="D44" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F44" s="1">
         <v>50</v>
@@ -2049,7 +2006,7 @@
         <v>1.4</v>
       </c>
       <c r="D45" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F45" s="1">
         <v>50</v>
@@ -2066,7 +2023,7 @@
         <v>1.4</v>
       </c>
       <c r="D46" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F46" s="1">
         <v>50</v>
@@ -2083,7 +2040,7 @@
         <v>1.4</v>
       </c>
       <c r="D47" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F47" s="1">
         <v>50</v>
@@ -2100,7 +2057,7 @@
         <v>1.4</v>
       </c>
       <c r="D48" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F48" s="1">
         <v>50</v>
@@ -2117,7 +2074,7 @@
         <v>1.4</v>
       </c>
       <c r="D49" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F49" s="1">
         <v>50</v>
@@ -2134,7 +2091,7 @@
         <v>1.4</v>
       </c>
       <c r="D50" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F50" s="1">
         <v>50</v>
@@ -2151,7 +2108,7 @@
         <v>1.4</v>
       </c>
       <c r="D51" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F51" s="1">
         <v>50</v>
@@ -2168,7 +2125,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D52" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F52" s="1">
         <v>50</v>
@@ -2185,7 +2142,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D53" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F53" s="1">
         <v>50</v>
@@ -2202,7 +2159,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D54" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F54" s="1">
         <v>50</v>
@@ -2219,7 +2176,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D55" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F55" s="1">
         <v>50</v>
@@ -2236,7 +2193,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D56" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F56" s="1">
         <v>50</v>
@@ -2253,7 +2210,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D57" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F57" s="1">
         <v>50</v>
@@ -2270,7 +2227,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D58" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F58" s="1">
         <v>50</v>
@@ -2287,7 +2244,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D59" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F59" s="1">
         <v>50</v>
@@ -2304,7 +2261,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D60" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F60" s="1">
         <v>50</v>
@@ -2321,7 +2278,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D61" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F61" s="1">
         <v>50</v>
@@ -2338,7 +2295,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D62" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F62" s="1">
         <v>50</v>
@@ -2355,7 +2312,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D63" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F63" s="1">
         <v>50</v>
@@ -2372,7 +2329,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D64" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F64" s="1">
         <v>50</v>
@@ -2389,7 +2346,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D65" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F65" s="1">
         <v>50</v>
@@ -2406,7 +2363,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D66" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F66" s="1">
         <v>50</v>
@@ -2423,7 +2380,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D67" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F67" s="1">
         <v>50</v>
@@ -2440,7 +2397,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D68" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F68" s="1">
         <v>50</v>
@@ -2457,7 +2414,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D69" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F69" s="1">
         <v>50</v>
@@ -2474,7 +2431,7 @@
         <v>7.6</v>
       </c>
       <c r="D70" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F70" s="1">
         <v>50</v>
@@ -2491,7 +2448,7 @@
         <v>7.6</v>
       </c>
       <c r="D71" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F71" s="1">
         <v>50</v>
@@ -2508,7 +2465,7 @@
         <v>7.6</v>
       </c>
       <c r="D72" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F72" s="1">
         <v>50</v>
@@ -2525,7 +2482,7 @@
         <v>7.6</v>
       </c>
       <c r="D73" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F73" s="1">
         <v>50</v>
@@ -2542,7 +2499,7 @@
         <v>7.6</v>
       </c>
       <c r="D74" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F74" s="1">
         <v>50</v>
@@ -2559,7 +2516,7 @@
         <v>7.6</v>
       </c>
       <c r="D75" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F75" s="1">
         <v>50</v>
@@ -2576,7 +2533,7 @@
         <v>7.6</v>
       </c>
       <c r="D76" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F76" s="1">
         <v>50</v>
@@ -2593,7 +2550,7 @@
         <v>7.6</v>
       </c>
       <c r="D77" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F77" s="1">
         <v>50</v>
@@ -2610,7 +2567,7 @@
         <v>7.6</v>
       </c>
       <c r="D78" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F78" s="1">
         <v>50</v>
@@ -2627,7 +2584,7 @@
         <v>7.6</v>
       </c>
       <c r="D79" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F79" s="1">
         <v>50</v>
@@ -2644,7 +2601,7 @@
         <v>7.6</v>
       </c>
       <c r="D80" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F80" s="1">
         <v>50</v>
@@ -2661,7 +2618,7 @@
         <v>7.6</v>
       </c>
       <c r="D81" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F81" s="1">
         <v>50</v>
@@ -2678,7 +2635,7 @@
         <v>7.6</v>
       </c>
       <c r="D82" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F82" s="1">
         <v>50</v>
@@ -2695,7 +2652,7 @@
         <v>7.6</v>
       </c>
       <c r="D83" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F83" s="1">
         <v>50</v>
@@ -2712,7 +2669,7 @@
         <v>7.6</v>
       </c>
       <c r="D84" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F84" s="1">
         <v>50</v>
@@ -2729,7 +2686,7 @@
         <v>7.6</v>
       </c>
       <c r="D85" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F85" s="1">
         <v>50</v>
@@ -2746,7 +2703,7 @@
         <v>7.6</v>
       </c>
       <c r="D86" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F86" s="1">
         <v>50</v>
@@ -2763,7 +2720,7 @@
         <v>7.6</v>
       </c>
       <c r="D87" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F87" s="1">
         <v>50</v>
@@ -2780,7 +2737,7 @@
         <v>7.6</v>
       </c>
       <c r="D88" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F88" s="1">
         <v>50</v>
@@ -2797,7 +2754,7 @@
         <v>7.6</v>
       </c>
       <c r="D89" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F89" s="1">
         <v>50</v>
@@ -2814,7 +2771,7 @@
         <v>7.6</v>
       </c>
       <c r="D90" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F90" s="1">
         <v>50</v>
@@ -2831,7 +2788,7 @@
         <v>7.6</v>
       </c>
       <c r="D91" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F91" s="1">
         <v>50</v>
@@ -2848,7 +2805,7 @@
         <v>7.6</v>
       </c>
       <c r="D92" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F92" s="1">
         <v>50</v>
@@ -2865,7 +2822,7 @@
         <v>3.1</v>
       </c>
       <c r="D93" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F93" s="1">
         <v>20</v>
@@ -2882,7 +2839,7 @@
         <v>3.1</v>
       </c>
       <c r="D94" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F94" s="1">
         <v>20</v>
@@ -2899,7 +2856,7 @@
         <v>3.1</v>
       </c>
       <c r="D95" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F95" s="1">
         <v>20</v>
@@ -2916,7 +2873,7 @@
         <v>3.1</v>
       </c>
       <c r="D96" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F96" s="1">
         <v>20</v>
@@ -2933,7 +2890,7 @@
         <v>3.1</v>
       </c>
       <c r="D97" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F97" s="1">
         <v>20</v>
@@ -2950,7 +2907,7 @@
         <v>3.1</v>
       </c>
       <c r="D98" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F98" s="1">
         <v>20</v>
@@ -2967,7 +2924,7 @@
         <v>3.1</v>
       </c>
       <c r="D99" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F99" s="1">
         <v>20</v>
@@ -2984,7 +2941,7 @@
         <v>3.1</v>
       </c>
       <c r="D100" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F100" s="1">
         <v>20</v>
@@ -3001,7 +2958,7 @@
         <v>3.1</v>
       </c>
       <c r="D101" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F101" s="1">
         <v>20</v>
@@ -3018,7 +2975,7 @@
         <v>3.1</v>
       </c>
       <c r="D102" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F102" s="1">
         <v>20</v>
@@ -3035,7 +2992,7 @@
         <v>3.1</v>
       </c>
       <c r="D103" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F103" s="1">
         <v>20</v>
@@ -3052,7 +3009,7 @@
         <v>3.1</v>
       </c>
       <c r="D104" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F104" s="1">
         <v>20</v>
@@ -3069,7 +3026,7 @@
         <v>3.1</v>
       </c>
       <c r="D105" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F105" s="1">
         <v>20</v>
@@ -3086,7 +3043,7 @@
         <v>3.1</v>
       </c>
       <c r="D106" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F106" s="1">
         <v>20</v>
@@ -3103,7 +3060,7 @@
         <v>3.1</v>
       </c>
       <c r="D107" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F107" s="1">
         <v>20</v>
@@ -3120,7 +3077,7 @@
         <v>3.1</v>
       </c>
       <c r="D108" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F108" s="1">
         <v>20</v>
@@ -3137,7 +3094,7 @@
         <v>3.1</v>
       </c>
       <c r="D109" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F109" s="1">
         <v>20</v>
@@ -3154,7 +3111,7 @@
         <v>3.1</v>
       </c>
       <c r="D110" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F110" s="1">
         <v>20</v>
@@ -3171,7 +3128,7 @@
         <v>3.1</v>
       </c>
       <c r="D111" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F111" s="1">
         <v>20</v>
@@ -3188,7 +3145,7 @@
         <v>3.1</v>
       </c>
       <c r="D112" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F112" s="1">
         <v>20</v>
@@ -3205,7 +3162,7 @@
         <v>3.1</v>
       </c>
       <c r="D113" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F113" s="1">
         <v>20</v>
@@ -3222,7 +3179,7 @@
         <v>3.1</v>
       </c>
       <c r="D114" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F114" s="1">
         <v>20</v>
@@ -3239,7 +3196,7 @@
         <v>3.1</v>
       </c>
       <c r="D115" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F115" s="1">
         <v>20</v>
@@ -3256,7 +3213,7 @@
         <v>3.1</v>
       </c>
       <c r="D116" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F116" s="1">
         <v>20</v>
@@ -3273,7 +3230,7 @@
         <v>3.1</v>
       </c>
       <c r="D117" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F117" s="1">
         <v>20</v>
@@ -3290,7 +3247,7 @@
         <v>3.1</v>
       </c>
       <c r="D118" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F118" s="1">
         <v>20</v>
@@ -3307,7 +3264,7 @@
         <v>3.1</v>
       </c>
       <c r="D119" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F119" s="1">
         <v>20</v>
@@ -3324,7 +3281,7 @@
         <v>3.1</v>
       </c>
       <c r="D120" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F120" s="1">
         <v>20</v>
@@ -3341,7 +3298,7 @@
         <v>3.1</v>
       </c>
       <c r="D121" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F121" s="1">
         <v>20</v>
@@ -3358,7 +3315,7 @@
         <v>3.1</v>
       </c>
       <c r="D122" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F122" s="1">
         <v>20</v>
@@ -3375,7 +3332,7 @@
         <v>3.1</v>
       </c>
       <c r="D123" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F123" s="1">
         <v>20</v>
@@ -3392,7 +3349,7 @@
         <v>3.1</v>
       </c>
       <c r="D124" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F124" s="1">
         <v>20</v>
@@ -3409,7 +3366,7 @@
         <v>3.1</v>
       </c>
       <c r="D125" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F125" s="1">
         <v>20</v>
@@ -3426,7 +3383,7 @@
         <v>3.1</v>
       </c>
       <c r="D126" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F126" s="1">
         <v>20</v>
@@ -3443,7 +3400,7 @@
         <v>3.1</v>
       </c>
       <c r="D127" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F127" s="1">
         <v>20</v>
@@ -3460,7 +3417,7 @@
         <v>3.1</v>
       </c>
       <c r="D128" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F128" s="1">
         <v>20</v>
@@ -3477,7 +3434,7 @@
         <v>3.1</v>
       </c>
       <c r="D129" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F129" s="1">
         <v>20</v>
@@ -3494,7 +3451,7 @@
         <v>3.1</v>
       </c>
       <c r="D130" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F130" s="1">
         <v>20</v>
@@ -3511,7 +3468,7 @@
         <v>3.1</v>
       </c>
       <c r="D131" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F131" s="1">
         <v>20</v>
@@ -3528,7 +3485,7 @@
         <v>3.1</v>
       </c>
       <c r="D132" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F132" s="1">
         <v>20</v>
@@ -3545,7 +3502,7 @@
         <v>3.1</v>
       </c>
       <c r="D133" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F133" s="1">
         <v>20</v>
@@ -3562,7 +3519,7 @@
         <v>3.1</v>
       </c>
       <c r="D134" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F134" s="1">
         <v>20</v>
@@ -3579,7 +3536,7 @@
         <v>7.5</v>
       </c>
       <c r="D135" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F135" s="1">
         <v>100</v>
@@ -3596,7 +3553,7 @@
         <v>7.5</v>
       </c>
       <c r="D136" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F136" s="1">
         <v>100</v>
@@ -3613,7 +3570,7 @@
         <v>7.5</v>
       </c>
       <c r="D137" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F137" s="1">
         <v>100</v>
@@ -3630,7 +3587,7 @@
         <v>7.5</v>
       </c>
       <c r="D138" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F138" s="1">
         <v>100</v>
@@ -3647,7 +3604,7 @@
         <v>7.4</v>
       </c>
       <c r="D139" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F139" s="1">
         <v>200</v>
@@ -3664,7 +3621,7 @@
         <v>7.3</v>
       </c>
       <c r="D140" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F140" s="1">
         <v>25</v>

</xml_diff>